<commit_message>
Results updated against 1000 randomized hierarchies
</commit_message>
<xml_diff>
--- a/data/HierConservation/results.xlsx
+++ b/data/HierConservation/results.xlsx
@@ -147,7 +147,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -170,8 +170,8 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -1196,7 +1196,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -1262,22 +1262,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.552139926289579</v>
+        <v>0.543135</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.432811960408211</v>
+        <v>0.416325</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.424956129971842</v>
+        <v>0.419712</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0.1371050111095</v>
+        <v>0.134032</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.00604490500864</v>
+        <v>0.00922317</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.00514933058702</v>
+        <v>0.0084504</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,27 +1286,27 @@
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B4-B5</f>
-        <v>0.165447374076474</v>
+        <v>0.174452300366053</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">C4-C5</f>
-        <v>0.133908511983053</v>
+        <v>0.150395472391263</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">D4-D5</f>
-        <v>0.173115787998895</v>
+        <v>0.178359917970737</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">E4-E5</f>
-        <v>0.06289242134332</v>
+        <v>0.06596543245282</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">F4-F5</f>
-        <v>0.00173383310718</v>
+        <v>-0.00144443188418</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">G4-G5</f>
-        <v>0.00208207437166</v>
+        <v>-0.00121899504132</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,22 +1337,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.538346457394842</v>
+        <v>0.535098</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.504315726915632</v>
+        <v>0.494541</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.406064993610947</v>
+        <v>0.403448</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>0.1919015269742</v>
+        <v>0.150666</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0</v>
+        <v>0.0140641</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0</v>
+        <v>0.0147694</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,27 +1361,27 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B8-B9</f>
-        <v>0.174417383763684</v>
+        <v>0.177665841158526</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">C8-C9</f>
-        <v>0.14916477228421</v>
+        <v>0.158939499199842</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">D8-D9</f>
-        <v>0.175845369503579</v>
+        <v>0.178462363114526</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">E8-E9</f>
-        <v>0.0918606662218</v>
+        <v>0.133096193196</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">F8-F9</f>
-        <v>0</v>
+        <v>-0.0140641</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">G8-G9</f>
-        <v>0</v>
+        <v>-0.0147694</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>